<commit_message>
UPDATE NOTULENSI, UPDATE PPJB,
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/NOTULENSI.xlsx
+++ b/RAPAT ANCOL/NOTULENSI.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwAmp\www\market_ancol - Copy\RAPAT ANCOL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwAmp\www\market_ancol\RAPAT ANCOL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="9 Sept 2015" sheetId="1" r:id="rId1"/>
     <sheet name="1 okt 2015" sheetId="2" r:id="rId2"/>
+    <sheet name="16 OKTOBER 2015" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t xml:space="preserve">   FORMAT : CEKLIS PEMBAYARAN, </t>
   </si>
@@ -190,6 +191,147 @@
   </si>
   <si>
     <t>MASTER STOK UPDATE EXCEL</t>
+  </si>
+  <si>
+    <t>BOOKING FEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANGGAL RENCANA </t>
+  </si>
+  <si>
+    <t>14 HARI KERJA SETELAH BOOKING FEE</t>
+  </si>
+  <si>
+    <t>ATAU TENTUKAN TANGGAL</t>
+  </si>
+  <si>
+    <t>RENCANA</t>
+  </si>
+  <si>
+    <t>MUNCUL DI ANGSURAN 1</t>
+  </si>
+  <si>
+    <t>MENGURANGI ANGSURAN 1</t>
+  </si>
+  <si>
+    <t>PENGISIAN TTS</t>
+  </si>
+  <si>
+    <t>OTOMATIS DICARI DAN DIISI DENGAN KODE BLOK YANG TERJUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANDA TERIMA DAN KUITANSI </t>
+  </si>
+  <si>
+    <t>TIDAK ADA TANDA TANGAN PEMBELI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORMAT PIUTANG SAMAIN AR </t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>DIILANGIN PT GRAHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP </t>
+  </si>
+  <si>
+    <t>TAMBAHIN SALES, GM PROPERTI 1, GM SALES</t>
+  </si>
+  <si>
+    <t>ALAMAT NPWP</t>
+  </si>
+  <si>
+    <t>DIHAPUS</t>
+  </si>
+  <si>
+    <t>ALAMAT RUMAH</t>
+  </si>
+  <si>
+    <t>CEKLIS -&gt; NGISI ALAMAT KORESPODENSI</t>
+  </si>
+  <si>
+    <t>ENTRI MANUAL</t>
+  </si>
+  <si>
+    <t>SALES, GM PROPERTI 1, GM SALES</t>
+  </si>
+  <si>
+    <t>2000000 ATAU ISI MANUAL</t>
+  </si>
+  <si>
+    <t>NILAI BOOKING FEE MASUK KE SP</t>
+  </si>
+  <si>
+    <t>LIHAT EXCEL AR CONDO TAB AR</t>
+  </si>
+  <si>
+    <t>JIKA CB36X</t>
+  </si>
+  <si>
+    <t>BALOON PAYMENT : PAKE RUMUS 5% UTK 1O BULAN, 15% UTK 12 BLN, 10% UTK 14 BLN, 70% SISANYA</t>
+  </si>
+  <si>
+    <t>MODUL</t>
+  </si>
+  <si>
+    <t>INPUTAN OTOMATIS CAPSLOK</t>
+  </si>
+  <si>
+    <t>POSISI UNIT TERJUAL</t>
+  </si>
+  <si>
+    <t>DIPAKE BUTTON UNTUK REFRESH</t>
+  </si>
+  <si>
+    <t>FORM PENJUALAN</t>
+  </si>
+  <si>
+    <t>BGB, REFERAL, MEMBER</t>
+  </si>
+  <si>
+    <t>172.16.32.42</t>
+  </si>
+  <si>
+    <t>10.8.12.111</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>4nc0l123!</t>
+  </si>
+  <si>
+    <t>PROPERTI-SALES</t>
+  </si>
+  <si>
+    <t>DAFTAR SPP</t>
+  </si>
+  <si>
+    <t>MASIH ADA LUAS TANAH</t>
+  </si>
+  <si>
+    <t>PPJB</t>
+  </si>
+  <si>
+    <t>TOTAL HARGA BELUM TO MONEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUITANSI PENJUALAN </t>
+  </si>
+  <si>
+    <t>POP UP DILEBARIN</t>
+  </si>
+  <si>
+    <t>CETAK KARTU PEMBELI</t>
+  </si>
+  <si>
+    <t>POP UP EROR</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -253,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -271,6 +413,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,6 +435,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:C24" totalsRowShown="0">
+  <autoFilter ref="A2:C24"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="MODUL"/>
+    <tableColumn id="2" name="KETERANGAN"/>
+    <tableColumn id="3" name="status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,20 +727,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -853,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -866,20 +1023,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1117,4 +1274,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
perbaikan sk harga dan print_spp.php
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/NOTULENSI.xlsx
+++ b/RAPAT ANCOL/NOTULENSI.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
   <si>
     <t xml:space="preserve">   FORMAT : CEKLIS PEMBAYARAN, </t>
   </si>
@@ -1281,7 +1281,7 @@
   <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,6 +1368,9 @@
       <c r="B9" t="s">
         <v>63</v>
       </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
perbaikan cetak kuitansi/kuitansi_print.php perbaikan cetak tanda_terima/tanda_terima_print.php perbaikan harga bangunan loadData perbaikan edit stok dan edit harga sk peraikan edit stok penjualan
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/NOTULENSI.xlsx
+++ b/RAPAT ANCOL/NOTULENSI.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwAmp\www\market_ancol\RAPAT ANCOL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="3"/>
   </bookViews>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
   <si>
     <t xml:space="preserve">   FORMAT : CEKLIS PEMBAYARAN, </t>
   </si>
@@ -335,12 +340,72 @@
   </si>
   <si>
     <t>Tampilan masih suka berbeda-beda</t>
+  </si>
+  <si>
+    <t>UMUR PIUTANG</t>
+  </si>
+  <si>
+    <t>0 TO 30</t>
+  </si>
+  <si>
+    <t>CASH IN</t>
+  </si>
+  <si>
+    <t>MASIH NGEBUG</t>
+  </si>
+  <si>
+    <t>NO TELP</t>
+  </si>
+  <si>
+    <t>FORMAT SURAT</t>
+  </si>
+  <si>
+    <t>DAFTAR KUITANSI</t>
+  </si>
+  <si>
+    <t>JUDUL PERBAIKI</t>
+  </si>
+  <si>
+    <t>MANUAL BOOK</t>
+  </si>
+  <si>
+    <t>SCREEN SHOOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAK AKSES </t>
+  </si>
+  <si>
+    <t>HAK AKSES PER MODUL</t>
+  </si>
+  <si>
+    <t>COLLECTION</t>
+  </si>
+  <si>
+    <t>BELUM DI CEK (PENAGIHAN , PERHITUNGAN DENDA, CREATE TAGIHAN)</t>
+  </si>
+  <si>
+    <t>NAMA PEJABAT, PEJABAT PPJB</t>
+  </si>
+  <si>
+    <t>UBAH DIDATABASE</t>
+  </si>
+  <si>
+    <t>MENU KARTU PEMBELI</t>
+  </si>
+  <si>
+    <t>HAPUS</t>
+  </si>
+  <si>
+    <t>MENU RENCANA REALISASI SELURUH BLOK</t>
+  </si>
+  <si>
+    <t>OTW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1526,13 +1591,13 @@
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1564,13 +1629,106 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
       <c r="E4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
       <c r="E5" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>